<commit_message>
Adding step to move final files
</commit_message>
<xml_diff>
--- a/EssilorLuxottica Projects/LUX - 7.0 - Report SAP Bank Files/Data/Config.xlsx
+++ b/EssilorLuxottica Projects/LUX - 7.0 - Report SAP Bank Files/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file-dallas\Process_Automation\Dept\RPA\GitHub Repos\UiPath\Automation Directory\Luxottica\LUX-2_Cybersource\4 - Business Unit Report\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\LRRBTUIPFSP100\Profiles\UIPATH_27\Desktop\GitHub\Luxottica-1\EssilorLuxottica Projects\LUX - 7.0 - Report SAP Bank Files\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393BEB24-C103-4314-9522-FA949E9FE6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17025" windowHeight="5235" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1545" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -248,9 +249,6 @@
     <t>strEmailDelayNotifications</t>
   </si>
   <si>
-    <t>LUX-2_BusinessUnitReport</t>
-  </si>
-  <si>
     <t>LUX-02_StrCopyFromPath</t>
   </si>
   <si>
@@ -288,12 +286,15 @@
   </si>
   <si>
     <t>LUX-02_StrReportsFolder</t>
+  </si>
+  <si>
+    <t>LUX-7.0-ReportSAPBankFiles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,6 +471,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -505,6 +523,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -680,11 +715,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -734,7 +769,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1800,7 +1835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3014,10 +3049,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -3066,7 +3101,7 @@
         <v>74</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3074,7 +3109,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3082,7 +3117,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -3091,7 +3126,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3099,7 +3134,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3107,7 +3142,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3115,7 +3150,7 @@
         <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3123,7 +3158,7 @@
         <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3131,7 +3166,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="10"/>
     </row>
@@ -3140,7 +3175,7 @@
         <v>58</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="7"/>
     </row>
@@ -3149,7 +3184,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="7"/>
     </row>
@@ -3179,10 +3214,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixing move files subprocess
</commit_message>
<xml_diff>
--- a/EssilorLuxottica Projects/LUX - 7.0 - Report SAP Bank Files/Data/Config.xlsx
+++ b/EssilorLuxottica Projects/LUX - 7.0 - Report SAP Bank Files/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\LRRBTUIPFSP100\Profiles\UIPATH_27\Desktop\GitHub\Luxottica-1\EssilorLuxottica Projects\LUX - 7.0 - Report SAP Bank Files\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393BEB24-C103-4314-9522-FA949E9FE6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8013CAB7-1022-42A0-9AB9-E421CF671956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1545" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -189,9 +189,6 @@
     <t>strSheetName</t>
   </si>
   <si>
-    <t>strWorkbookPassword</t>
-  </si>
-  <si>
     <t>strEmailServer</t>
   </si>
   <si>
@@ -231,71 +228,62 @@
     <t>strProcessRoot</t>
   </si>
   <si>
-    <t>ALL_ProcessRoot</t>
-  </si>
-  <si>
     <t>strSubProcessRoot</t>
   </si>
   <si>
-    <t>ALL_SubProcessRoot</t>
-  </si>
-  <si>
     <t>strComponentRoot</t>
   </si>
   <si>
-    <t>ALL_ComponentRoot</t>
-  </si>
-  <si>
-    <t>strEmailDelayNotifications</t>
-  </si>
-  <si>
-    <t>LUX-02_StrCopyFromPath</t>
-  </si>
-  <si>
-    <t>LUX-02_StrCopyFromName</t>
-  </si>
-  <si>
-    <t>LUX-02_StrCopyToPath</t>
-  </si>
-  <si>
-    <t>LUX-02_StrCopyToName</t>
-  </si>
-  <si>
-    <t>LUX-02_StrWorkbookFilePath</t>
-  </si>
-  <si>
-    <t>LUX-02_StrWorkbookFileName</t>
-  </si>
-  <si>
-    <t>LUX-02_StrSheetName</t>
-  </si>
-  <si>
-    <t>LUX-02_StrWorkbookPassword</t>
-  </si>
-  <si>
-    <t>LUX-02_StrEmailCCAddress</t>
-  </si>
-  <si>
-    <t>LUX-02_StrHistoryPathMergeReport</t>
-  </si>
-  <si>
-    <t>LUX-02_StrEmailCyberSource</t>
-  </si>
-  <si>
-    <t>strReportsFolder</t>
-  </si>
-  <si>
-    <t>LUX-02_StrReportsFolder</t>
-  </si>
-  <si>
     <t>LUX-7.0-ReportSAPBankFiles</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrEmalBankFiles</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrCopyFromPath</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrCopyFromName</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrCopyToPath</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrCopyToName</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrWorkbookFilePath</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrWorkbookFileName</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrSheetName</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrEmailCCAddress</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrHistoryPathMergeReport</t>
+  </si>
+  <si>
+    <t>strEmailBankFiles</t>
+  </si>
+  <si>
+    <t>\\LRRBTUIPFSP100\Profiles\UIPATH_27\Desktop\GitHub\Luxottica-1\EssilorLuxottica Projects\Components\</t>
+  </si>
+  <si>
+    <t>\\LRRBTUIPFSP100\Profiles\UIPATH_27\Desktop\GitHub\Luxottica-1\EssilorLuxottica Projects\LUX - 7.0 - Report SAP Bank Files\Subprocesses\</t>
+  </si>
+  <si>
+    <t>\\LRRBTUIPFSP100\Profiles\UIPATH_27\Desktop\GitHub\Luxottica-1\EssilorLuxottica Projects\LUX - 7.0 - Report SAP Bank Files\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -327,12 +315,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF485056"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -358,9 +340,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -375,8 +357,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -719,7 +700,7 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -769,7 +750,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -793,23 +774,23 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
         <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>30</v>
@@ -817,7 +798,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <v>465</v>
@@ -825,7 +806,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="9" t="b">
         <v>1</v>
@@ -836,38 +817,57 @@
         <v>54</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>66</v>
-      </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1829,8 +1829,13 @@
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{70354B90-D474-47B1-ACDB-0E6645C19023}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{439FFF84-321E-496A-BB6E-A67C52124D5A}"/>
+    <hyperlink ref="B15" r:id="rId3" xr:uid="{672CD8AB-F73E-4A35-9590-C9F6E860CD55}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3053,7 +3058,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3098,10 +3103,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3109,7 +3114,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3117,7 +3122,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -3126,7 +3131,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3134,7 +3139,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3142,15 +3147,15 @@
         <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>80</v>
+      <c r="B8" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3158,68 +3163,30 @@
         <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>79</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>58</v>
+      <c r="A11" t="s">
+        <v>66</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="7"/>
+        <v>80</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding reporting process changes
</commit_message>
<xml_diff>
--- a/EssilorLuxottica Projects/LUX - 7.0 - Report SAP Bank Files/Data/Config.xlsx
+++ b/EssilorLuxottica Projects/LUX - 7.0 - Report SAP Bank Files/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\LRRBTUIPFSP100\Profiles\UIPATH_27\Desktop\GitHub\Luxottica-1\EssilorLuxottica Projects\LUX - 7.0 - Report SAP Bank Files\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8013CAB7-1022-42A0-9AB9-E421CF671956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0785EC4D-5684-487E-87BB-1DAD57A99F47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="2985" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -192,24 +192,12 @@
     <t>strEmailServer</t>
   </si>
   <si>
-    <t>smtp.gmail.com</t>
-  </si>
-  <si>
     <t>strEmailCCAddress</t>
   </si>
   <si>
-    <t>strEmailTaxOpsAddress</t>
-  </si>
-  <si>
     <t>intDaysToDelete</t>
   </si>
   <si>
-    <t>intEmailPort</t>
-  </si>
-  <si>
-    <t>carlos.cortez@essilorusa.com</t>
-  </si>
-  <si>
     <t>boolHeaders</t>
   </si>
   <si>
@@ -237,9 +225,6 @@
     <t>LUX-7.0-ReportSAPBankFiles</t>
   </si>
   <si>
-    <t>Ess.LUX-7.0_StrEmalBankFiles</t>
-  </si>
-  <si>
     <t>Ess.LUX-7.0_StrCopyFromPath</t>
   </si>
   <si>
@@ -277,6 +262,18 @@
   </si>
   <si>
     <t>\\LRRBTUIPFSP100\Profiles\UIPATH_27\Desktop\GitHub\Luxottica-1\EssilorLuxottica Projects\LUX - 7.0 - Report SAP Bank Files\</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_EmailPort</t>
+  </si>
+  <si>
+    <t>strEmailPort</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_EmailServer</t>
+  </si>
+  <si>
+    <t>Ess.LUX-7.0_StrEmailBankFiles</t>
   </si>
 </sst>
 </file>
@@ -699,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -750,7 +747,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -772,41 +769,24 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10">
-        <v>465</v>
-      </c>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B11" s="9" t="b">
         <v>1</v>
@@ -817,40 +797,40 @@
         <v>54</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3057,8 +3037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3103,10 +3083,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3114,7 +3094,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3122,7 +3102,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -3131,7 +3111,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3139,7 +3119,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3147,7 +3127,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3155,7 +3135,7 @@
         <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3163,27 +3143,41 @@
         <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>